<commit_message>
Add standalone POST script and SSL verification improvements
- Added post_mtr_data.py: Independent script for JSON uploads to database
  * Certificate-based authentication
  * Batch processing of JSON files
  * SSL verification configuration options
  * Interactive menu system
  * Comprehensive error handling and logging

- Updated pdf_processor_new prompt.py: SSL verification improvements
- Added test_heat_numbers.py: Testing utility
- Added MTR.TXT: 40 heat numbers for testing
- Reorganized Sample json files: Renamed for better organization
- Cleaned up unused MTR JSON files
</commit_message>
<xml_diff>
--- a/Sample json/NEW_.xlsx
+++ b/Sample json/NEW_.xlsx
@@ -420,7 +420,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CV42"/>
+  <dimension ref="A1:CV43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -953,7 +953,7 @@
       </c>
       <c r="AA3" s="1" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.003</t>
         </is>
       </c>
       <c r="AB3" s="1" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="AV3" s="1" t="inlineStr">
         <is>
-          <t>0.0004</t>
+          <t>0.003</t>
         </is>
       </c>
       <c r="AW3" s="1" t="inlineStr">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="BM3" s="1" t="inlineStr">
         <is>
-          <t>0.0004</t>
+          <t>0.003</t>
         </is>
       </c>
       <c r="BN3" s="1" t="inlineStr">
@@ -1895,7 +1895,7 @@
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>78200</t>
+          <t>60000</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>86800</t>
+          <t>75000</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
@@ -2083,7 +2083,7 @@
       </c>
       <c r="AU6" s="1" t="inlineStr">
         <is>
-          <t>0.030</t>
+          <t>0.028</t>
         </is>
       </c>
       <c r="AV6" s="1" t="inlineStr">
@@ -2164,7 +2164,7 @@
       </c>
       <c r="BL6" s="1" t="inlineStr">
         <is>
-          <t>0.030</t>
+          <t>0.029</t>
         </is>
       </c>
       <c r="BM6" s="1" t="inlineStr">
@@ -2705,27 +2705,27 @@
       </c>
       <c r="Y8" s="1" t="inlineStr">
         <is>
+          <t>0.002</t>
+        </is>
+      </c>
+      <c r="Z8" s="1" t="inlineStr">
+        <is>
           <t>0.036</t>
         </is>
       </c>
-      <c r="Z8" s="1" t="inlineStr">
+      <c r="AA8" s="1" t="inlineStr">
+        <is>
+          <t>0.0004</t>
+        </is>
+      </c>
+      <c r="AB8" s="1" t="inlineStr">
+        <is>
+          <t>0.0078</t>
+        </is>
+      </c>
+      <c r="AC8" s="1" t="inlineStr">
         <is>
           <t>0.0016</t>
-        </is>
-      </c>
-      <c r="AA8" s="1" t="inlineStr">
-        <is>
-          <t>0.0004</t>
-        </is>
-      </c>
-      <c r="AB8" s="1" t="inlineStr">
-        <is>
-          <t>0.0078</t>
-        </is>
-      </c>
-      <c r="AC8" s="1" t="inlineStr">
-        <is>
-          <t>0.000</t>
         </is>
       </c>
       <c r="AD8" s="1" t="inlineStr">
@@ -2794,27 +2794,27 @@
       </c>
       <c r="AT8" s="1" t="inlineStr">
         <is>
+          <t>0.001</t>
+        </is>
+      </c>
+      <c r="AU8" s="1" t="inlineStr">
+        <is>
           <t>0.036</t>
         </is>
       </c>
-      <c r="AU8" s="1" t="inlineStr">
+      <c r="AV8" s="1" t="inlineStr">
+        <is>
+          <t>0.0001</t>
+        </is>
+      </c>
+      <c r="AW8" s="1" t="inlineStr">
+        <is>
+          <t>0.0080</t>
+        </is>
+      </c>
+      <c r="AX8" s="1" t="inlineStr">
         <is>
           <t>0.0014</t>
-        </is>
-      </c>
-      <c r="AV8" s="1" t="inlineStr">
-        <is>
-          <t>0.0001</t>
-        </is>
-      </c>
-      <c r="AW8" s="1" t="inlineStr">
-        <is>
-          <t>0.0080</t>
-        </is>
-      </c>
-      <c r="AX8" s="1" t="inlineStr">
-        <is>
-          <t>0.000</t>
         </is>
       </c>
       <c r="AY8" s="1" t="inlineStr"/>
@@ -2875,27 +2875,27 @@
       </c>
       <c r="BK8" s="1" t="inlineStr">
         <is>
+          <t>0.001</t>
+        </is>
+      </c>
+      <c r="BL8" s="1" t="inlineStr">
+        <is>
           <t>0.036</t>
         </is>
       </c>
-      <c r="BL8" s="1" t="inlineStr">
+      <c r="BM8" s="1" t="inlineStr">
+        <is>
+          <t>0.0001</t>
+        </is>
+      </c>
+      <c r="BN8" s="1" t="inlineStr">
+        <is>
+          <t>0.0091</t>
+        </is>
+      </c>
+      <c r="BO8" s="1" t="inlineStr">
         <is>
           <t>0.0012</t>
-        </is>
-      </c>
-      <c r="BM8" s="1" t="inlineStr">
-        <is>
-          <t>0.0001</t>
-        </is>
-      </c>
-      <c r="BN8" s="1" t="inlineStr">
-        <is>
-          <t>0.0091</t>
-        </is>
-      </c>
-      <c r="BO8" s="1" t="inlineStr">
-        <is>
-          <t>0.000</t>
         </is>
       </c>
       <c r="BP8" s="1" t="inlineStr">
@@ -3016,49 +3016,49 @@
       </c>
       <c r="R9" s="1" t="inlineStr">
         <is>
+          <t>0.029</t>
+        </is>
+      </c>
+      <c r="S9" s="1" t="inlineStr">
+        <is>
+          <t>0.264</t>
+        </is>
+      </c>
+      <c r="T9" s="1" t="inlineStr">
+        <is>
+          <t>0.017</t>
+        </is>
+      </c>
+      <c r="U9" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="V9" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="W9" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="X9" s="1" t="inlineStr">
+        <is>
+          <t>0.040</t>
+        </is>
+      </c>
+      <c r="Y9" s="1" t="inlineStr">
+        <is>
+          <t>0.067</t>
+        </is>
+      </c>
+      <c r="Z9" s="1" t="inlineStr">
+        <is>
           <t>0.032</t>
         </is>
       </c>
-      <c r="S9" s="1" t="inlineStr">
-        <is>
-          <t>0.264</t>
-        </is>
-      </c>
-      <c r="T9" s="1" t="inlineStr">
-        <is>
-          <t>0.017</t>
-        </is>
-      </c>
-      <c r="U9" s="1" t="inlineStr">
-        <is>
-          <t>0.03</t>
-        </is>
-      </c>
-      <c r="V9" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="W9" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="X9" s="1" t="inlineStr">
-        <is>
-          <t>0.040</t>
-        </is>
-      </c>
-      <c r="Y9" s="1" t="inlineStr">
-        <is>
-          <t>0.067</t>
-        </is>
-      </c>
-      <c r="Z9" s="1" t="inlineStr">
-        <is>
-          <t>0.029</t>
-        </is>
-      </c>
       <c r="AA9" s="1" t="inlineStr">
         <is>
           <t>0.0003</t>
@@ -3074,9 +3074,17 @@
           <t>0.0026</t>
         </is>
       </c>
-      <c r="AD9" s="1" t="inlineStr"/>
+      <c r="AD9" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
       <c r="AE9" s="1" t="inlineStr"/>
-      <c r="AF9" s="1" t="inlineStr"/>
+      <c r="AF9" s="1" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
       <c r="AG9" s="1" t="inlineStr"/>
       <c r="AH9" s="1" t="inlineStr"/>
       <c r="AI9" s="1" t="inlineStr">
@@ -3101,47 +3109,47 @@
       </c>
       <c r="AM9" s="1" t="inlineStr">
         <is>
+          <t>0.028</t>
+        </is>
+      </c>
+      <c r="AN9" s="1" t="inlineStr">
+        <is>
+          <t>0.262</t>
+        </is>
+      </c>
+      <c r="AO9" s="1" t="inlineStr">
+        <is>
+          <t>0.017</t>
+        </is>
+      </c>
+      <c r="AP9" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AQ9" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AR9" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AS9" s="1" t="inlineStr">
+        <is>
+          <t>0.040</t>
+        </is>
+      </c>
+      <c r="AT9" s="1" t="inlineStr">
+        <is>
+          <t>0.069</t>
+        </is>
+      </c>
+      <c r="AU9" s="1" t="inlineStr">
+        <is>
           <t>0.033</t>
-        </is>
-      </c>
-      <c r="AN9" s="1" t="inlineStr">
-        <is>
-          <t>0.262</t>
-        </is>
-      </c>
-      <c r="AO9" s="1" t="inlineStr">
-        <is>
-          <t>0.017</t>
-        </is>
-      </c>
-      <c r="AP9" s="1" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="AQ9" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="AR9" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="AS9" s="1" t="inlineStr">
-        <is>
-          <t>0.040</t>
-        </is>
-      </c>
-      <c r="AT9" s="1" t="inlineStr">
-        <is>
-          <t>0.069</t>
-        </is>
-      </c>
-      <c r="AU9" s="1" t="inlineStr">
-        <is>
-          <t>0.028</t>
         </is>
       </c>
       <c r="AV9" s="1" t="inlineStr">
@@ -3182,49 +3190,49 @@
       </c>
       <c r="BD9" s="1" t="inlineStr">
         <is>
+          <t>0.029</t>
+        </is>
+      </c>
+      <c r="BE9" s="1" t="inlineStr">
+        <is>
+          <t>0.264</t>
+        </is>
+      </c>
+      <c r="BF9" s="1" t="inlineStr">
+        <is>
+          <t>0.017</t>
+        </is>
+      </c>
+      <c r="BG9" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="BH9" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="BI9" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="BJ9" s="1" t="inlineStr">
+        <is>
+          <t>0.040</t>
+        </is>
+      </c>
+      <c r="BK9" s="1" t="inlineStr">
+        <is>
+          <t>0.069</t>
+        </is>
+      </c>
+      <c r="BL9" s="1" t="inlineStr">
+        <is>
           <t>0.032</t>
         </is>
       </c>
-      <c r="BE9" s="1" t="inlineStr">
-        <is>
-          <t>0.264</t>
-        </is>
-      </c>
-      <c r="BF9" s="1" t="inlineStr">
-        <is>
-          <t>0.017</t>
-        </is>
-      </c>
-      <c r="BG9" s="1" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="BH9" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="BI9" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="BJ9" s="1" t="inlineStr">
-        <is>
-          <t>0.040</t>
-        </is>
-      </c>
-      <c r="BK9" s="1" t="inlineStr">
-        <is>
-          <t>0.069</t>
-        </is>
-      </c>
-      <c r="BL9" s="1" t="inlineStr">
-        <is>
-          <t>0.029</t>
-        </is>
-      </c>
       <c r="BM9" s="1" t="inlineStr">
         <is>
           <t>0.0003</t>
@@ -3240,12 +3248,28 @@
           <t>0.0024</t>
         </is>
       </c>
-      <c r="BP9" s="1" t="inlineStr"/>
+      <c r="BP9" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
       <c r="BQ9" s="1" t="inlineStr"/>
-      <c r="BR9" s="1" t="inlineStr"/>
+      <c r="BR9" s="1" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
       <c r="BS9" s="1" t="inlineStr"/>
-      <c r="BT9" s="1" t="inlineStr"/>
-      <c r="BU9" s="1" t="inlineStr"/>
+      <c r="BT9" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="BU9" s="1" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
       <c r="BV9" s="1" t="inlineStr"/>
       <c r="BW9" s="1" t="inlineStr"/>
       <c r="BX9" s="1" t="inlineStr"/>
@@ -3408,12 +3432,12 @@
       </c>
       <c r="AB10" s="1" t="inlineStr">
         <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="AC10" s="1" t="inlineStr">
+        <is>
           <t>0.006</t>
-        </is>
-      </c>
-      <c r="AC10" s="1" t="inlineStr">
-        <is>
-          <t>0.012</t>
         </is>
       </c>
       <c r="AD10" s="1" t="inlineStr">
@@ -3501,12 +3525,12 @@
       </c>
       <c r="AW10" s="1" t="inlineStr">
         <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="AX10" s="1" t="inlineStr">
+        <is>
           <t>0.0036</t>
-        </is>
-      </c>
-      <c r="AX10" s="1" t="inlineStr">
-        <is>
-          <t>0.012</t>
         </is>
       </c>
       <c r="AY10" s="1" t="inlineStr"/>
@@ -3582,12 +3606,12 @@
       </c>
       <c r="BN10" s="1" t="inlineStr">
         <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="BO10" s="1" t="inlineStr">
+        <is>
           <t>0.0033</t>
-        </is>
-      </c>
-      <c r="BO10" s="1" t="inlineStr">
-        <is>
-          <t>0.012</t>
         </is>
       </c>
       <c r="BP10" s="1" t="inlineStr">
@@ -4148,9 +4172,17 @@
           <t>0.12</t>
         </is>
       </c>
-      <c r="AD12" s="1" t="inlineStr"/>
+      <c r="AD12" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
       <c r="AE12" s="1" t="inlineStr"/>
-      <c r="AF12" s="1" t="inlineStr"/>
+      <c r="AF12" s="1" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
       <c r="AG12" s="1" t="inlineStr"/>
       <c r="AH12" s="1" t="inlineStr"/>
       <c r="AI12" s="1" t="inlineStr">
@@ -4314,12 +4346,28 @@
           <t>0.12</t>
         </is>
       </c>
-      <c r="BP12" s="1" t="inlineStr"/>
+      <c r="BP12" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
       <c r="BQ12" s="1" t="inlineStr"/>
-      <c r="BR12" s="1" t="inlineStr"/>
+      <c r="BR12" s="1" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
       <c r="BS12" s="1" t="inlineStr"/>
-      <c r="BT12" s="1" t="inlineStr"/>
-      <c r="BU12" s="1" t="inlineStr"/>
+      <c r="BT12" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="BU12" s="1" t="inlineStr">
+        <is>
+          <t>0.34</t>
+        </is>
+      </c>
       <c r="BV12" s="1" t="inlineStr"/>
       <c r="BW12" s="1" t="inlineStr"/>
       <c r="BX12" s="1" t="inlineStr"/>
@@ -14900,6 +14948,260 @@
       <c r="CU42" s="1" t="inlineStr"/>
       <c r="CV42" s="1" t="inlineStr"/>
     </row>
+    <row r="43">
+      <c r="A43" s="1" t="inlineStr"/>
+      <c r="B43" s="1" t="inlineStr">
+        <is>
+          <t>60752</t>
+        </is>
+      </c>
+      <c r="C43" s="1" t="inlineStr">
+        <is>
+          <t>06/06/2025</t>
+        </is>
+      </c>
+      <c r="D43" s="1" t="inlineStr">
+        <is>
+          <t>Tenaris Tamsa</t>
+        </is>
+      </c>
+      <c r="E43" s="1" t="inlineStr">
+        <is>
+          <t>Mexico</t>
+        </is>
+      </c>
+      <c r="F43" s="1" t="inlineStr"/>
+      <c r="G43" s="1" t="inlineStr">
+        <is>
+          <t>64200</t>
+        </is>
+      </c>
+      <c r="H43" s="1" t="inlineStr">
+        <is>
+          <t>Psi</t>
+        </is>
+      </c>
+      <c r="I43" s="1" t="inlineStr">
+        <is>
+          <t>84000</t>
+        </is>
+      </c>
+      <c r="J43" s="1" t="inlineStr">
+        <is>
+          <t>Psi</t>
+        </is>
+      </c>
+      <c r="K43" s="1" t="inlineStr"/>
+      <c r="L43" s="1" t="inlineStr"/>
+      <c r="M43" s="1" t="inlineStr"/>
+      <c r="N43" s="1" t="inlineStr">
+        <is>
+          <t>.120</t>
+        </is>
+      </c>
+      <c r="O43" s="1" t="inlineStr">
+        <is>
+          <t>1.260</t>
+        </is>
+      </c>
+      <c r="P43" s="1" t="inlineStr">
+        <is>
+          <t>.008</t>
+        </is>
+      </c>
+      <c r="Q43" s="1" t="inlineStr">
+        <is>
+          <t>.001</t>
+        </is>
+      </c>
+      <c r="R43" s="1" t="inlineStr">
+        <is>
+          <t>.014</t>
+        </is>
+      </c>
+      <c r="S43" s="1" t="inlineStr">
+        <is>
+          <t>.250</t>
+        </is>
+      </c>
+      <c r="T43" s="1" t="inlineStr">
+        <is>
+          <t>.0030</t>
+        </is>
+      </c>
+      <c r="U43" s="1" t="inlineStr">
+        <is>
+          <t>.070</t>
+        </is>
+      </c>
+      <c r="V43" s="1" t="inlineStr">
+        <is>
+          <t>.120</t>
+        </is>
+      </c>
+      <c r="W43" s="1" t="inlineStr">
+        <is>
+          <t>.066</t>
+        </is>
+      </c>
+      <c r="X43" s="1" t="inlineStr">
+        <is>
+          <t>.150</t>
+        </is>
+      </c>
+      <c r="Y43" s="1" t="inlineStr">
+        <is>
+          <t>.0260</t>
+        </is>
+      </c>
+      <c r="Z43" s="1" t="inlineStr">
+        <is>
+          <t>.0003</t>
+        </is>
+      </c>
+      <c r="AA43" s="1" t="inlineStr"/>
+      <c r="AB43" s="1" t="inlineStr"/>
+      <c r="AC43" s="1" t="inlineStr"/>
+      <c r="AD43" s="1" t="inlineStr">
+        <is>
+          <t>.40</t>
+        </is>
+      </c>
+      <c r="AE43" s="1" t="inlineStr"/>
+      <c r="AF43" s="1" t="inlineStr">
+        <is>
+          <t>.34</t>
+        </is>
+      </c>
+      <c r="AG43" s="1" t="inlineStr"/>
+      <c r="AH43" s="1" t="inlineStr"/>
+      <c r="AI43" s="1" t="inlineStr">
+        <is>
+          <t>.120</t>
+        </is>
+      </c>
+      <c r="AJ43" s="1" t="inlineStr">
+        <is>
+          <t>1.290</t>
+        </is>
+      </c>
+      <c r="AK43" s="1" t="inlineStr">
+        <is>
+          <t>.012</t>
+        </is>
+      </c>
+      <c r="AL43" s="1" t="inlineStr">
+        <is>
+          <t>.001</t>
+        </is>
+      </c>
+      <c r="AM43" s="1" t="inlineStr">
+        <is>
+          <t>.010</t>
+        </is>
+      </c>
+      <c r="AN43" s="1" t="inlineStr">
+        <is>
+          <t>.280</t>
+        </is>
+      </c>
+      <c r="AO43" s="1" t="inlineStr">
+        <is>
+          <t>&lt;. 0100</t>
+        </is>
+      </c>
+      <c r="AP43" s="1" t="inlineStr">
+        <is>
+          <t>.080</t>
+        </is>
+      </c>
+      <c r="AQ43" s="1" t="inlineStr">
+        <is>
+          <t>.130</t>
+        </is>
+      </c>
+      <c r="AR43" s="1" t="inlineStr">
+        <is>
+          <t>.070</t>
+        </is>
+      </c>
+      <c r="AS43" s="1" t="inlineStr">
+        <is>
+          <t>.160</t>
+        </is>
+      </c>
+      <c r="AT43" s="1" t="inlineStr">
+        <is>
+          <t>.0300</t>
+        </is>
+      </c>
+      <c r="AU43" s="1" t="inlineStr">
+        <is>
+          <t>&lt;. 0005</t>
+        </is>
+      </c>
+      <c r="AV43" s="1" t="inlineStr"/>
+      <c r="AW43" s="1" t="inlineStr"/>
+      <c r="AX43" s="1" t="inlineStr"/>
+      <c r="AY43" s="1" t="inlineStr"/>
+      <c r="AZ43" s="1" t="inlineStr"/>
+      <c r="BA43" s="1" t="inlineStr"/>
+      <c r="BB43" s="1" t="inlineStr"/>
+      <c r="BC43" s="1" t="inlineStr"/>
+      <c r="BD43" s="1" t="inlineStr"/>
+      <c r="BE43" s="1" t="inlineStr"/>
+      <c r="BF43" s="1" t="inlineStr"/>
+      <c r="BG43" s="1" t="inlineStr"/>
+      <c r="BH43" s="1" t="inlineStr"/>
+      <c r="BI43" s="1" t="inlineStr"/>
+      <c r="BJ43" s="1" t="inlineStr"/>
+      <c r="BK43" s="1" t="inlineStr"/>
+      <c r="BL43" s="1" t="inlineStr"/>
+      <c r="BM43" s="1" t="inlineStr"/>
+      <c r="BN43" s="1" t="inlineStr"/>
+      <c r="BO43" s="1" t="inlineStr"/>
+      <c r="BP43" s="1" t="inlineStr">
+        <is>
+          <t>.41</t>
+        </is>
+      </c>
+      <c r="BQ43" s="1" t="inlineStr"/>
+      <c r="BR43" s="1" t="inlineStr">
+        <is>
+          <t>.35</t>
+        </is>
+      </c>
+      <c r="BS43" s="1" t="inlineStr"/>
+      <c r="BT43" s="1" t="inlineStr"/>
+      <c r="BU43" s="1" t="inlineStr"/>
+      <c r="BV43" s="1" t="inlineStr"/>
+      <c r="BW43" s="1" t="inlineStr"/>
+      <c r="BX43" s="1" t="inlineStr"/>
+      <c r="BY43" s="1" t="inlineStr"/>
+      <c r="BZ43" s="1" t="inlineStr"/>
+      <c r="CA43" s="1" t="inlineStr"/>
+      <c r="CB43" s="1" t="inlineStr"/>
+      <c r="CC43" s="1" t="inlineStr"/>
+      <c r="CD43" s="1" t="inlineStr"/>
+      <c r="CE43" s="1" t="inlineStr"/>
+      <c r="CF43" s="1" t="inlineStr"/>
+      <c r="CG43" s="1" t="inlineStr"/>
+      <c r="CH43" s="1" t="inlineStr"/>
+      <c r="CI43" s="1" t="inlineStr"/>
+      <c r="CJ43" s="1" t="inlineStr"/>
+      <c r="CK43" s="1" t="inlineStr"/>
+      <c r="CL43" s="1" t="inlineStr"/>
+      <c r="CM43" s="1" t="inlineStr"/>
+      <c r="CN43" s="1" t="inlineStr"/>
+      <c r="CO43" s="1" t="inlineStr"/>
+      <c r="CP43" s="1" t="inlineStr"/>
+      <c r="CQ43" s="1" t="inlineStr"/>
+      <c r="CR43" s="1" t="inlineStr"/>
+      <c r="CS43" s="1" t="inlineStr"/>
+      <c r="CT43" s="1" t="inlineStr"/>
+      <c r="CU43" s="1" t="inlineStr"/>
+      <c r="CV43" s="1" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: centralize token generation in decryption, wire DEFAULT_AUTH_TOKEN getters; add CompanyMTRFileID propagation/enforcement; add API invalid-response debug logging; add post_mtr_data uploader
</commit_message>
<xml_diff>
--- a/Sample json/NEW_.xlsx
+++ b/Sample json/NEW_.xlsx
@@ -953,7 +953,7 @@
       </c>
       <c r="AA3" s="1" t="inlineStr">
         <is>
-          <t>0.003</t>
+          <t>0.0002</t>
         </is>
       </c>
       <c r="AB3" s="1" t="inlineStr">
@@ -1038,7 +1038,7 @@
       </c>
       <c r="AV3" s="1" t="inlineStr">
         <is>
-          <t>0.003</t>
+          <t>0.0004</t>
         </is>
       </c>
       <c r="AW3" s="1" t="inlineStr">
@@ -1119,7 +1119,7 @@
       </c>
       <c r="BM3" s="1" t="inlineStr">
         <is>
-          <t>0.003</t>
+          <t>0.0004</t>
         </is>
       </c>
       <c r="BN3" s="1" t="inlineStr">
@@ -1265,32 +1265,32 @@
       </c>
       <c r="U4" s="1" t="inlineStr">
         <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="V4" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="W4" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="X4" s="1" t="inlineStr">
+        <is>
           <t>0.26</t>
         </is>
       </c>
-      <c r="V4" s="1" t="inlineStr">
+      <c r="Y4" s="1" t="inlineStr">
+        <is>
+          <t>0.004</t>
+        </is>
+      </c>
+      <c r="Z4" s="1" t="inlineStr">
         <is>
           <t>0.09</t>
-        </is>
-      </c>
-      <c r="W4" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="X4" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="Y4" s="1" t="inlineStr">
-        <is>
-          <t>0.004</t>
-        </is>
-      </c>
-      <c r="Z4" s="1" t="inlineStr">
-        <is>
-          <t>0.030</t>
         </is>
       </c>
       <c r="AA4" s="1" t="inlineStr">
@@ -1358,32 +1358,32 @@
       </c>
       <c r="AP4" s="1" t="inlineStr">
         <is>
+          <t>0.31</t>
+        </is>
+      </c>
+      <c r="AQ4" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="AR4" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="AS4" s="1" t="inlineStr">
+        <is>
           <t>0.24</t>
         </is>
       </c>
-      <c r="AQ4" s="1" t="inlineStr">
+      <c r="AT4" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="AU4" s="1" t="inlineStr">
         <is>
           <t>0.09</t>
-        </is>
-      </c>
-      <c r="AR4" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="AS4" s="1" t="inlineStr">
-        <is>
-          <t>0.31</t>
-        </is>
-      </c>
-      <c r="AT4" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="AU4" s="1" t="inlineStr">
-        <is>
-          <t>0.031</t>
         </is>
       </c>
       <c r="AV4" s="1" t="inlineStr">
@@ -1439,32 +1439,32 @@
       </c>
       <c r="BG4" s="1" t="inlineStr">
         <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="BH4" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="BI4" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="BJ4" s="1" t="inlineStr">
+        <is>
           <t>0.25</t>
         </is>
       </c>
-      <c r="BH4" s="1" t="inlineStr">
+      <c r="BK4" s="1" t="inlineStr">
+        <is>
+          <t>0.004</t>
+        </is>
+      </c>
+      <c r="BL4" s="1" t="inlineStr">
         <is>
           <t>0.09</t>
-        </is>
-      </c>
-      <c r="BI4" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="BJ4" s="1" t="inlineStr">
-        <is>
-          <t>0.30</t>
-        </is>
-      </c>
-      <c r="BK4" s="1" t="inlineStr">
-        <is>
-          <t>0.004</t>
-        </is>
-      </c>
-      <c r="BL4" s="1" t="inlineStr">
-        <is>
-          <t>0.030</t>
         </is>
       </c>
       <c r="BM4" s="1" t="inlineStr">
@@ -1658,12 +1658,12 @@
       </c>
       <c r="AB5" s="1" t="inlineStr">
         <is>
+          <t>0.0027</t>
+        </is>
+      </c>
+      <c r="AC5" s="1" t="inlineStr">
+        <is>
           <t>0.006</t>
-        </is>
-      </c>
-      <c r="AC5" s="1" t="inlineStr">
-        <is>
-          <t>0.0027</t>
         </is>
       </c>
       <c r="AD5" s="1" t="inlineStr"/>
@@ -1743,12 +1743,12 @@
       </c>
       <c r="AW5" s="1" t="inlineStr">
         <is>
+          <t>0.0027</t>
+        </is>
+      </c>
+      <c r="AX5" s="1" t="inlineStr">
+        <is>
           <t>0.005</t>
-        </is>
-      </c>
-      <c r="AX5" s="1" t="inlineStr">
-        <is>
-          <t>0.0027</t>
         </is>
       </c>
       <c r="AY5" s="1" t="inlineStr"/>
@@ -1824,12 +1824,12 @@
       </c>
       <c r="BN5" s="1" t="inlineStr">
         <is>
+          <t>0.0030</t>
+        </is>
+      </c>
+      <c r="BO5" s="1" t="inlineStr">
+        <is>
           <t>0.005</t>
-        </is>
-      </c>
-      <c r="BO5" s="1" t="inlineStr">
-        <is>
-          <t>0.0030</t>
         </is>
       </c>
       <c r="BP5" s="1" t="inlineStr"/>
@@ -1895,7 +1895,7 @@
       </c>
       <c r="G6" s="1" t="inlineStr">
         <is>
-          <t>60000</t>
+          <t>78200</t>
         </is>
       </c>
       <c r="H6" s="1" t="inlineStr">
@@ -1905,7 +1905,7 @@
       </c>
       <c r="I6" s="1" t="inlineStr">
         <is>
-          <t>75000</t>
+          <t>86800</t>
         </is>
       </c>
       <c r="J6" s="1" t="inlineStr">
@@ -2246,7 +2246,7 @@
       </c>
       <c r="D7" s="1" t="inlineStr">
         <is>
-          <t>Berg Pipe Panama City Corp</t>
+          <t>Berg Pipe-Panama City, FL</t>
         </is>
       </c>
       <c r="E7" s="1" t="inlineStr">
@@ -2668,59 +2668,51 @@
           <t>0.006</t>
         </is>
       </c>
-      <c r="R8" s="1" t="inlineStr">
+      <c r="R8" s="1" t="inlineStr"/>
+      <c r="S8" s="1" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="T8" s="1" t="inlineStr"/>
+      <c r="U8" s="1" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="V8" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="W8" s="1" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="X8" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="Y8" s="1" t="inlineStr">
+        <is>
+          <t>0.009</t>
+        </is>
+      </c>
+      <c r="Z8" s="1" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AA8" s="1" t="inlineStr">
         <is>
           <t>0.002</t>
         </is>
       </c>
-      <c r="S8" s="1" t="inlineStr">
-        <is>
-          <t>0.23</t>
-        </is>
-      </c>
-      <c r="T8" s="1" t="inlineStr">
-        <is>
-          <t>0.002</t>
-        </is>
-      </c>
-      <c r="U8" s="1" t="inlineStr">
-        <is>
-          <t>0.14</t>
-        </is>
-      </c>
-      <c r="V8" s="1" t="inlineStr">
-        <is>
-          <t>0.05</t>
-        </is>
-      </c>
-      <c r="W8" s="1" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="X8" s="1" t="inlineStr">
-        <is>
-          <t>0.08</t>
-        </is>
-      </c>
-      <c r="Y8" s="1" t="inlineStr">
-        <is>
-          <t>0.002</t>
-        </is>
-      </c>
-      <c r="Z8" s="1" t="inlineStr">
+      <c r="AB8" s="1" t="inlineStr">
         <is>
           <t>0.036</t>
-        </is>
-      </c>
-      <c r="AA8" s="1" t="inlineStr">
-        <is>
-          <t>0.0004</t>
-        </is>
-      </c>
-      <c r="AB8" s="1" t="inlineStr">
-        <is>
-          <t>0.0078</t>
         </is>
       </c>
       <c r="AC8" s="1" t="inlineStr">
@@ -2757,59 +2749,51 @@
           <t>0.004</t>
         </is>
       </c>
-      <c r="AM8" s="1" t="inlineStr">
+      <c r="AM8" s="1" t="inlineStr"/>
+      <c r="AN8" s="1" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="AO8" s="1" t="inlineStr"/>
+      <c r="AP8" s="1" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="AQ8" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AR8" s="1" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="AS8" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AT8" s="1" t="inlineStr">
+        <is>
+          <t>0.006</t>
+        </is>
+      </c>
+      <c r="AU8" s="1" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="AV8" s="1" t="inlineStr">
         <is>
           <t>0.001</t>
         </is>
       </c>
-      <c r="AN8" s="1" t="inlineStr">
-        <is>
-          <t>0.23</t>
-        </is>
-      </c>
-      <c r="AO8" s="1" t="inlineStr">
-        <is>
-          <t>0.002</t>
-        </is>
-      </c>
-      <c r="AP8" s="1" t="inlineStr">
-        <is>
-          <t>0.15</t>
-        </is>
-      </c>
-      <c r="AQ8" s="1" t="inlineStr">
-        <is>
-          <t>0.05</t>
-        </is>
-      </c>
-      <c r="AR8" s="1" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="AS8" s="1" t="inlineStr">
-        <is>
-          <t>0.08</t>
-        </is>
-      </c>
-      <c r="AT8" s="1" t="inlineStr">
-        <is>
-          <t>0.001</t>
-        </is>
-      </c>
-      <c r="AU8" s="1" t="inlineStr">
+      <c r="AW8" s="1" t="inlineStr">
         <is>
           <t>0.036</t>
-        </is>
-      </c>
-      <c r="AV8" s="1" t="inlineStr">
-        <is>
-          <t>0.0001</t>
-        </is>
-      </c>
-      <c r="AW8" s="1" t="inlineStr">
-        <is>
-          <t>0.0080</t>
         </is>
       </c>
       <c r="AX8" s="1" t="inlineStr">
@@ -2838,59 +2822,51 @@
           <t>0.005</t>
         </is>
       </c>
-      <c r="BD8" s="1" t="inlineStr">
+      <c r="BD8" s="1" t="inlineStr"/>
+      <c r="BE8" s="1" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="BF8" s="1" t="inlineStr"/>
+      <c r="BG8" s="1" t="inlineStr">
+        <is>
+          <t>0.15</t>
+        </is>
+      </c>
+      <c r="BH8" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="BI8" s="1" t="inlineStr">
+        <is>
+          <t>0.08</t>
+        </is>
+      </c>
+      <c r="BJ8" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="BK8" s="1" t="inlineStr">
+        <is>
+          <t>0.006</t>
+        </is>
+      </c>
+      <c r="BL8" s="1" t="inlineStr">
+        <is>
+          <t>0.000</t>
+        </is>
+      </c>
+      <c r="BM8" s="1" t="inlineStr">
         <is>
           <t>0.001</t>
         </is>
       </c>
-      <c r="BE8" s="1" t="inlineStr">
-        <is>
-          <t>0.23</t>
-        </is>
-      </c>
-      <c r="BF8" s="1" t="inlineStr">
-        <is>
-          <t>0.002</t>
-        </is>
-      </c>
-      <c r="BG8" s="1" t="inlineStr">
-        <is>
-          <t>0.15</t>
-        </is>
-      </c>
-      <c r="BH8" s="1" t="inlineStr">
-        <is>
-          <t>0.05</t>
-        </is>
-      </c>
-      <c r="BI8" s="1" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="BJ8" s="1" t="inlineStr">
-        <is>
-          <t>0.08</t>
-        </is>
-      </c>
-      <c r="BK8" s="1" t="inlineStr">
-        <is>
-          <t>0.001</t>
-        </is>
-      </c>
-      <c r="BL8" s="1" t="inlineStr">
+      <c r="BN8" s="1" t="inlineStr">
         <is>
           <t>0.036</t>
-        </is>
-      </c>
-      <c r="BM8" s="1" t="inlineStr">
-        <is>
-          <t>0.0001</t>
-        </is>
-      </c>
-      <c r="BN8" s="1" t="inlineStr">
-        <is>
-          <t>0.0091</t>
         </is>
       </c>
       <c r="BO8" s="1" t="inlineStr">
@@ -3074,17 +3050,9 @@
           <t>0.0026</t>
         </is>
       </c>
-      <c r="AD9" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
+      <c r="AD9" s="1" t="inlineStr"/>
       <c r="AE9" s="1" t="inlineStr"/>
-      <c r="AF9" s="1" t="inlineStr">
-        <is>
-          <t>0.11</t>
-        </is>
-      </c>
+      <c r="AF9" s="1" t="inlineStr"/>
       <c r="AG9" s="1" t="inlineStr"/>
       <c r="AH9" s="1" t="inlineStr"/>
       <c r="AI9" s="1" t="inlineStr">
@@ -3248,28 +3216,12 @@
           <t>0.0024</t>
         </is>
       </c>
-      <c r="BP9" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
+      <c r="BP9" s="1" t="inlineStr"/>
       <c r="BQ9" s="1" t="inlineStr"/>
-      <c r="BR9" s="1" t="inlineStr">
-        <is>
-          <t>0.11</t>
-        </is>
-      </c>
+      <c r="BR9" s="1" t="inlineStr"/>
       <c r="BS9" s="1" t="inlineStr"/>
-      <c r="BT9" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="BU9" s="1" t="inlineStr">
-        <is>
-          <t>0.12</t>
-        </is>
-      </c>
+      <c r="BT9" s="1" t="inlineStr"/>
+      <c r="BU9" s="1" t="inlineStr"/>
       <c r="BV9" s="1" t="inlineStr"/>
       <c r="BW9" s="1" t="inlineStr"/>
       <c r="BX9" s="1" t="inlineStr"/>
@@ -3432,12 +3384,12 @@
       </c>
       <c r="AB10" s="1" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.006</t>
         </is>
       </c>
       <c r="AC10" s="1" t="inlineStr">
         <is>
-          <t>0.006</t>
+          <t>0.012</t>
         </is>
       </c>
       <c r="AD10" s="1" t="inlineStr">
@@ -3525,12 +3477,12 @@
       </c>
       <c r="AW10" s="1" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.0036</t>
         </is>
       </c>
       <c r="AX10" s="1" t="inlineStr">
         <is>
-          <t>0.0036</t>
+          <t>0.012</t>
         </is>
       </c>
       <c r="AY10" s="1" t="inlineStr"/>
@@ -3606,12 +3558,12 @@
       </c>
       <c r="BN10" s="1" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.0033</t>
         </is>
       </c>
       <c r="BO10" s="1" t="inlineStr">
         <is>
-          <t>0.0033</t>
+          <t>0.012</t>
         </is>
       </c>
       <c r="BP10" s="1" t="inlineStr">
@@ -4172,17 +4124,9 @@
           <t>0.12</t>
         </is>
       </c>
-      <c r="AD12" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
+      <c r="AD12" s="1" t="inlineStr"/>
       <c r="AE12" s="1" t="inlineStr"/>
-      <c r="AF12" s="1" t="inlineStr">
-        <is>
-          <t>0.34</t>
-        </is>
-      </c>
+      <c r="AF12" s="1" t="inlineStr"/>
       <c r="AG12" s="1" t="inlineStr"/>
       <c r="AH12" s="1" t="inlineStr"/>
       <c r="AI12" s="1" t="inlineStr">
@@ -4346,28 +4290,12 @@
           <t>0.12</t>
         </is>
       </c>
-      <c r="BP12" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
+      <c r="BP12" s="1" t="inlineStr"/>
       <c r="BQ12" s="1" t="inlineStr"/>
-      <c r="BR12" s="1" t="inlineStr">
-        <is>
-          <t>0.34</t>
-        </is>
-      </c>
+      <c r="BR12" s="1" t="inlineStr"/>
       <c r="BS12" s="1" t="inlineStr"/>
-      <c r="BT12" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="BU12" s="1" t="inlineStr">
-        <is>
-          <t>0.34</t>
-        </is>
-      </c>
+      <c r="BT12" s="1" t="inlineStr"/>
+      <c r="BU12" s="1" t="inlineStr"/>
       <c r="BV12" s="1" t="inlineStr"/>
       <c r="BW12" s="1" t="inlineStr"/>
       <c r="BX12" s="1" t="inlineStr"/>
@@ -5140,47 +5068,47 @@
       </c>
       <c r="R15" s="1" t="inlineStr">
         <is>
+          <t>0.031</t>
+        </is>
+      </c>
+      <c r="S15" s="1" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="T15" s="1" t="inlineStr">
+        <is>
+          <t>0.013</t>
+        </is>
+      </c>
+      <c r="U15" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="V15" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="W15" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="X15" s="1" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+      <c r="Y15" s="1" t="inlineStr">
+        <is>
+          <t>0.072</t>
+        </is>
+      </c>
+      <c r="Z15" s="1" t="inlineStr">
+        <is>
           <t>0.030</t>
-        </is>
-      </c>
-      <c r="S15" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="T15" s="1" t="inlineStr">
-        <is>
-          <t>0.013</t>
-        </is>
-      </c>
-      <c r="U15" s="1" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="V15" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="W15" s="1" t="inlineStr">
-        <is>
-          <t>0.03</t>
-        </is>
-      </c>
-      <c r="X15" s="1" t="inlineStr">
-        <is>
-          <t>0.003</t>
-        </is>
-      </c>
-      <c r="Y15" s="1" t="inlineStr">
-        <is>
-          <t>0.072</t>
-        </is>
-      </c>
-      <c r="Z15" s="1" t="inlineStr">
-        <is>
-          <t>0.031</t>
         </is>
       </c>
       <c r="AA15" s="1" t="inlineStr">
@@ -5524,12 +5452,12 @@
       </c>
       <c r="AB16" s="1" t="inlineStr">
         <is>
+          <t>0.0040</t>
+        </is>
+      </c>
+      <c r="AC16" s="1" t="inlineStr">
+        <is>
           <t>0.007</t>
-        </is>
-      </c>
-      <c r="AC16" s="1" t="inlineStr">
-        <is>
-          <t>0.0040</t>
         </is>
       </c>
       <c r="AD16" s="1" t="inlineStr"/>
@@ -5609,12 +5537,12 @@
       </c>
       <c r="AW16" s="1" t="inlineStr">
         <is>
+          <t>0.0039</t>
+        </is>
+      </c>
+      <c r="AX16" s="1" t="inlineStr">
+        <is>
           <t>0.005</t>
-        </is>
-      </c>
-      <c r="AX16" s="1" t="inlineStr">
-        <is>
-          <t>0.0039</t>
         </is>
       </c>
       <c r="AY16" s="1" t="inlineStr"/>
@@ -5690,12 +5618,12 @@
       </c>
       <c r="BN16" s="1" t="inlineStr">
         <is>
+          <t>0.0039</t>
+        </is>
+      </c>
+      <c r="BO16" s="1" t="inlineStr">
+        <is>
           <t>0.006</t>
-        </is>
-      </c>
-      <c r="BO16" s="1" t="inlineStr">
-        <is>
-          <t>0.0039</t>
         </is>
       </c>
       <c r="BP16" s="1" t="inlineStr"/>
@@ -6810,52 +6738,52 @@
       </c>
       <c r="R20" s="1" t="inlineStr">
         <is>
+          <t>0.029</t>
+        </is>
+      </c>
+      <c r="S20" s="1" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="T20" s="1" t="inlineStr">
+        <is>
+          <t>0.014</t>
+        </is>
+      </c>
+      <c r="U20" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="V20" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="W20" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="X20" s="1" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+      <c r="Y20" s="1" t="inlineStr">
+        <is>
+          <t>0.067</t>
+        </is>
+      </c>
+      <c r="Z20" s="1" t="inlineStr">
+        <is>
           <t>0.031</t>
         </is>
       </c>
-      <c r="S20" s="1" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="T20" s="1" t="inlineStr">
-        <is>
-          <t>0.014</t>
-        </is>
-      </c>
-      <c r="U20" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="V20" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="W20" s="1" t="inlineStr">
-        <is>
-          <t>0.02</t>
-        </is>
-      </c>
-      <c r="X20" s="1" t="inlineStr">
-        <is>
-          <t>0.003</t>
-        </is>
-      </c>
-      <c r="Y20" s="1" t="inlineStr">
-        <is>
-          <t>0.067</t>
-        </is>
-      </c>
-      <c r="Z20" s="1" t="inlineStr">
-        <is>
-          <t>0.029</t>
-        </is>
-      </c>
       <c r="AA20" s="1" t="inlineStr">
         <is>
-          <t>0.0002</t>
+          <t>0.002</t>
         </is>
       </c>
       <c r="AB20" s="1" t="inlineStr">
@@ -6865,7 +6793,7 @@
       </c>
       <c r="AC20" s="1" t="inlineStr">
         <is>
-          <t>0.002</t>
+          <t>0.0034</t>
         </is>
       </c>
       <c r="AD20" s="1" t="inlineStr"/>
@@ -6895,54 +6823,54 @@
       </c>
       <c r="AM20" s="1" t="inlineStr">
         <is>
+          <t>0.030</t>
+        </is>
+      </c>
+      <c r="AN20" s="1" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="AO20" s="1" t="inlineStr">
+        <is>
+          <t>0.015</t>
+        </is>
+      </c>
+      <c r="AP20" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AQ20" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AR20" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AS20" s="1" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+      <c r="AT20" s="1" t="inlineStr">
+        <is>
+          <t>0.070</t>
+        </is>
+      </c>
+      <c r="AU20" s="1" t="inlineStr">
+        <is>
           <t>0.031</t>
         </is>
       </c>
-      <c r="AN20" s="1" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="AO20" s="1" t="inlineStr">
-        <is>
-          <t>0.015</t>
-        </is>
-      </c>
-      <c r="AP20" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="AQ20" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="AR20" s="1" t="inlineStr">
-        <is>
-          <t>0.03</t>
-        </is>
-      </c>
-      <c r="AS20" s="1" t="inlineStr">
+      <c r="AV20" s="1" t="inlineStr">
         <is>
           <t>0.003</t>
         </is>
       </c>
-      <c r="AT20" s="1" t="inlineStr">
-        <is>
-          <t>0.070</t>
-        </is>
-      </c>
-      <c r="AU20" s="1" t="inlineStr">
-        <is>
-          <t>0.030</t>
-        </is>
-      </c>
-      <c r="AV20" s="1" t="inlineStr">
-        <is>
-          <t>0.0002</t>
-        </is>
-      </c>
       <c r="AW20" s="1" t="inlineStr">
         <is>
           <t>0.006</t>
@@ -6950,7 +6878,7 @@
       </c>
       <c r="AX20" s="1" t="inlineStr">
         <is>
-          <t>0.003</t>
+          <t>0.0034</t>
         </is>
       </c>
       <c r="AY20" s="1" t="inlineStr"/>
@@ -6976,54 +6904,54 @@
       </c>
       <c r="BD20" s="1" t="inlineStr">
         <is>
+          <t>0.029</t>
+        </is>
+      </c>
+      <c r="BE20" s="1" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="BF20" s="1" t="inlineStr">
+        <is>
+          <t>0.015</t>
+        </is>
+      </c>
+      <c r="BG20" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="BH20" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="BI20" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="BJ20" s="1" t="inlineStr">
+        <is>
+          <t>0.003</t>
+        </is>
+      </c>
+      <c r="BK20" s="1" t="inlineStr">
+        <is>
+          <t>0.070</t>
+        </is>
+      </c>
+      <c r="BL20" s="1" t="inlineStr">
+        <is>
           <t>0.031</t>
         </is>
       </c>
-      <c r="BE20" s="1" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="BF20" s="1" t="inlineStr">
-        <is>
-          <t>0.015</t>
-        </is>
-      </c>
-      <c r="BG20" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="BH20" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
-      <c r="BI20" s="1" t="inlineStr">
-        <is>
-          <t>0.03</t>
-        </is>
-      </c>
-      <c r="BJ20" s="1" t="inlineStr">
+      <c r="BM20" s="1" t="inlineStr">
         <is>
           <t>0.003</t>
         </is>
       </c>
-      <c r="BK20" s="1" t="inlineStr">
-        <is>
-          <t>0.070</t>
-        </is>
-      </c>
-      <c r="BL20" s="1" t="inlineStr">
-        <is>
-          <t>0.029</t>
-        </is>
-      </c>
-      <c r="BM20" s="1" t="inlineStr">
-        <is>
-          <t>0.0002</t>
-        </is>
-      </c>
       <c r="BN20" s="1" t="inlineStr">
         <is>
           <t>0.005</t>
@@ -7031,7 +6959,7 @@
       </c>
       <c r="BO20" s="1" t="inlineStr">
         <is>
-          <t>0.003</t>
+          <t>0.0030</t>
         </is>
       </c>
       <c r="BP20" s="1" t="inlineStr"/>
@@ -7097,17 +7025,17 @@
       </c>
       <c r="G21" s="1" t="inlineStr">
         <is>
+          <t>84100</t>
+        </is>
+      </c>
+      <c r="H21" s="1" t="inlineStr">
+        <is>
+          <t>psi</t>
+        </is>
+      </c>
+      <c r="I21" s="1" t="inlineStr">
+        <is>
           <t>75400</t>
-        </is>
-      </c>
-      <c r="H21" s="1" t="inlineStr">
-        <is>
-          <t>psi</t>
-        </is>
-      </c>
-      <c r="I21" s="1" t="inlineStr">
-        <is>
-          <t>84100</t>
         </is>
       </c>
       <c r="J21" s="1" t="inlineStr">
@@ -7493,32 +7421,32 @@
       </c>
       <c r="U22" s="1" t="inlineStr">
         <is>
-          <t>0.30</t>
+          <t>0.03</t>
         </is>
       </c>
       <c r="V22" s="1" t="inlineStr">
         <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="W22" s="1" t="inlineStr">
+        <is>
           <t>0.03</t>
         </is>
       </c>
-      <c r="W22" s="1" t="inlineStr">
-        <is>
-          <t>0.01</t>
-        </is>
-      </c>
       <c r="X22" s="1" t="inlineStr">
         <is>
-          <t>0.03</t>
+          <t>0.004</t>
         </is>
       </c>
       <c r="Y22" s="1" t="inlineStr">
         <is>
-          <t>0.004</t>
+          <t>0.028</t>
         </is>
       </c>
       <c r="Z22" s="1" t="inlineStr">
         <is>
-          <t>0.028</t>
+          <t>0.015</t>
         </is>
       </c>
       <c r="AA22" s="1" t="inlineStr">
@@ -7528,12 +7456,12 @@
       </c>
       <c r="AB22" s="1" t="inlineStr">
         <is>
-          <t>0.015</t>
+          <t>0.006</t>
         </is>
       </c>
       <c r="AC22" s="1" t="inlineStr">
         <is>
-          <t>0.0027</t>
+          <t>0.005</t>
         </is>
       </c>
       <c r="AD22" s="1" t="inlineStr"/>
@@ -7613,12 +7541,12 @@
       </c>
       <c r="AW22" s="1" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.006</t>
         </is>
       </c>
       <c r="AX22" s="1" t="inlineStr">
         <is>
-          <t>0.0026</t>
+          <t>0.005</t>
         </is>
       </c>
       <c r="AY22" s="1" t="inlineStr"/>
@@ -7694,12 +7622,12 @@
       </c>
       <c r="BN22" s="1" t="inlineStr">
         <is>
-          <t>0.12</t>
+          <t>0.006</t>
         </is>
       </c>
       <c r="BO22" s="1" t="inlineStr">
         <is>
-          <t>0.0029</t>
+          <t>0.005</t>
         </is>
       </c>
       <c r="BP22" s="1" t="inlineStr"/>
@@ -7837,12 +7765,12 @@
       </c>
       <c r="W23" s="1" t="inlineStr">
         <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="X23" s="1" t="inlineStr">
+        <is>
           <t>0.006</t>
-        </is>
-      </c>
-      <c r="X23" s="1" t="inlineStr">
-        <is>
-          <t>0.03</t>
         </is>
       </c>
       <c r="Y23" s="1" t="inlineStr">
@@ -7922,12 +7850,12 @@
       </c>
       <c r="AR23" s="1" t="inlineStr">
         <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AS23" s="1" t="inlineStr">
+        <is>
           <t>0.007</t>
-        </is>
-      </c>
-      <c r="AS23" s="1" t="inlineStr">
-        <is>
-          <t>0.03</t>
         </is>
       </c>
       <c r="AT23" s="1" t="inlineStr">
@@ -8003,12 +7931,12 @@
       </c>
       <c r="BI23" s="1" t="inlineStr">
         <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="BJ23" s="1" t="inlineStr">
+        <is>
           <t>0.007</t>
-        </is>
-      </c>
-      <c r="BJ23" s="1" t="inlineStr">
-        <is>
-          <t>0.03</t>
         </is>
       </c>
       <c r="BK23" s="1" t="inlineStr">
@@ -9193,42 +9121,42 @@
       </c>
       <c r="S27" s="1" t="inlineStr">
         <is>
+          <t>0.004</t>
+        </is>
+      </c>
+      <c r="T27" s="1" t="inlineStr">
+        <is>
           <t>0.016</t>
         </is>
       </c>
-      <c r="T27" s="1" t="inlineStr">
-        <is>
-          <t>0.004</t>
-        </is>
-      </c>
       <c r="U27" s="1" t="inlineStr">
         <is>
+          <t>0.031</t>
+        </is>
+      </c>
+      <c r="V27" s="1" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="W27" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="X27" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="Y27" s="1" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+      <c r="Z27" s="1" t="inlineStr">
+        <is>
           <t>0.10</t>
-        </is>
-      </c>
-      <c r="V27" s="1" t="inlineStr">
-        <is>
-          <t>0.26</t>
-        </is>
-      </c>
-      <c r="W27" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="X27" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="Y27" s="1" t="inlineStr">
-        <is>
-          <t>0.031</t>
-        </is>
-      </c>
-      <c r="Z27" s="1" t="inlineStr">
-        <is>
-          <t>0.016</t>
         </is>
       </c>
       <c r="AA27" s="1" t="inlineStr">
@@ -9286,42 +9214,42 @@
       </c>
       <c r="AN27" s="1" t="inlineStr">
         <is>
+          <t>0.004</t>
+        </is>
+      </c>
+      <c r="AO27" s="1" t="inlineStr">
+        <is>
           <t>0.016</t>
         </is>
       </c>
-      <c r="AO27" s="1" t="inlineStr">
-        <is>
-          <t>0.004</t>
-        </is>
-      </c>
       <c r="AP27" s="1" t="inlineStr">
         <is>
+          <t>0.032</t>
+        </is>
+      </c>
+      <c r="AQ27" s="1" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="AR27" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AS27" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="AT27" s="1" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="AU27" s="1" t="inlineStr">
+        <is>
           <t>0.09</t>
-        </is>
-      </c>
-      <c r="AQ27" s="1" t="inlineStr">
-        <is>
-          <t>0.25</t>
-        </is>
-      </c>
-      <c r="AR27" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="AS27" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="AT27" s="1" t="inlineStr">
-        <is>
-          <t>0.032</t>
-        </is>
-      </c>
-      <c r="AU27" s="1" t="inlineStr">
-        <is>
-          <t>0.016</t>
         </is>
       </c>
       <c r="AV27" s="1" t="inlineStr">
@@ -9367,42 +9295,42 @@
       </c>
       <c r="BE27" s="1" t="inlineStr">
         <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="BF27" s="1" t="inlineStr">
+        <is>
           <t>0.015</t>
         </is>
       </c>
-      <c r="BF27" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
       <c r="BG27" s="1" t="inlineStr">
         <is>
+          <t>0.032</t>
+        </is>
+      </c>
+      <c r="BH27" s="1" t="inlineStr">
+        <is>
+          <t>0.30</t>
+        </is>
+      </c>
+      <c r="BI27" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="BJ27" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="BK27" s="1" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="BL27" s="1" t="inlineStr">
+        <is>
           <t>0.09</t>
-        </is>
-      </c>
-      <c r="BH27" s="1" t="inlineStr">
-        <is>
-          <t>0.25</t>
-        </is>
-      </c>
-      <c r="BI27" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="BJ27" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="BK27" s="1" t="inlineStr">
-        <is>
-          <t>0.032</t>
-        </is>
-      </c>
-      <c r="BL27" s="1" t="inlineStr">
-        <is>
-          <t>0.015</t>
         </is>
       </c>
       <c r="BM27" s="1" t="inlineStr">
@@ -9559,55 +9487,59 @@
       </c>
       <c r="S28" s="1" t="inlineStr">
         <is>
+          <t>0.028</t>
+        </is>
+      </c>
+      <c r="T28" s="1" t="inlineStr">
+        <is>
           <t>0.015</t>
         </is>
       </c>
-      <c r="T28" s="1" t="inlineStr">
+      <c r="U28" s="1" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="V28" s="1" t="inlineStr">
+        <is>
+          <t>0.13</t>
+        </is>
+      </c>
+      <c r="W28" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="X28" s="1" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="Y28" s="1" t="inlineStr">
         <is>
           <t>0.005</t>
         </is>
       </c>
-      <c r="U28" s="1" t="inlineStr">
-        <is>
-          <t>0.13</t>
-        </is>
-      </c>
-      <c r="V28" s="1" t="inlineStr">
+      <c r="Z28" s="1" t="inlineStr">
+        <is>
+          <t>0.016</t>
+        </is>
+      </c>
+      <c r="AA28" s="1" t="inlineStr">
         <is>
           <t>0.0001</t>
         </is>
       </c>
-      <c r="W28" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="X28" s="1" t="inlineStr">
-        <is>
-          <t>0.028</t>
-        </is>
-      </c>
-      <c r="Y28" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="Z28" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="AA28" s="1" t="inlineStr">
+      <c r="AB28" s="1" t="inlineStr">
         <is>
           <t>0.006</t>
         </is>
       </c>
-      <c r="AB28" s="1" t="inlineStr">
+      <c r="AC28" s="1" t="inlineStr">
         <is>
           <t>0.0010</t>
         </is>
       </c>
-      <c r="AC28" s="1" t="inlineStr"/>
       <c r="AD28" s="1" t="inlineStr">
         <is>
           <t>0.160</t>
@@ -9648,55 +9580,59 @@
       </c>
       <c r="AN28" s="1" t="inlineStr">
         <is>
+          <t>0.028</t>
+        </is>
+      </c>
+      <c r="AO28" s="1" t="inlineStr">
+        <is>
           <t>0.015</t>
         </is>
       </c>
-      <c r="AO28" s="1" t="inlineStr">
+      <c r="AP28" s="1" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="AQ28" s="1" t="inlineStr">
+        <is>
+          <t>0.14</t>
+        </is>
+      </c>
+      <c r="AR28" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="AS28" s="1" t="inlineStr">
+        <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="AT28" s="1" t="inlineStr">
         <is>
           <t>0.005</t>
         </is>
       </c>
-      <c r="AP28" s="1" t="inlineStr">
-        <is>
-          <t>0.14</t>
-        </is>
-      </c>
-      <c r="AQ28" s="1" t="inlineStr">
+      <c r="AU28" s="1" t="inlineStr">
+        <is>
+          <t>0.016</t>
+        </is>
+      </c>
+      <c r="AV28" s="1" t="inlineStr">
         <is>
           <t>0.0001</t>
         </is>
       </c>
-      <c r="AR28" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="AS28" s="1" t="inlineStr">
-        <is>
-          <t>0.028</t>
-        </is>
-      </c>
-      <c r="AT28" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="AU28" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="AV28" s="1" t="inlineStr">
+      <c r="AW28" s="1" t="inlineStr">
         <is>
           <t>0.006</t>
         </is>
       </c>
-      <c r="AW28" s="1" t="inlineStr">
+      <c r="AX28" s="1" t="inlineStr">
         <is>
           <t>0.0010</t>
         </is>
       </c>
-      <c r="AX28" s="1" t="inlineStr"/>
       <c r="AY28" s="1" t="inlineStr"/>
       <c r="AZ28" s="1" t="inlineStr">
         <is>
@@ -9725,55 +9661,59 @@
       </c>
       <c r="BE28" s="1" t="inlineStr">
         <is>
+          <t>0.027</t>
+        </is>
+      </c>
+      <c r="BF28" s="1" t="inlineStr">
+        <is>
           <t>0.014</t>
         </is>
       </c>
-      <c r="BF28" s="1" t="inlineStr">
+      <c r="BG28" s="1" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="BH28" s="1" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="BI28" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="BJ28" s="1" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="BK28" s="1" t="inlineStr">
         <is>
           <t>0.005</t>
         </is>
       </c>
-      <c r="BG28" s="1" t="inlineStr">
-        <is>
-          <t>0.12</t>
-        </is>
-      </c>
-      <c r="BH28" s="1" t="inlineStr">
+      <c r="BL28" s="1" t="inlineStr">
+        <is>
+          <t>0.016</t>
+        </is>
+      </c>
+      <c r="BM28" s="1" t="inlineStr">
         <is>
           <t>0.0001</t>
         </is>
       </c>
-      <c r="BI28" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="BJ28" s="1" t="inlineStr">
-        <is>
-          <t>0.027</t>
-        </is>
-      </c>
-      <c r="BK28" s="1" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="BL28" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="BM28" s="1" t="inlineStr">
+      <c r="BN28" s="1" t="inlineStr">
         <is>
           <t>0.005</t>
         </is>
       </c>
-      <c r="BN28" s="1" t="inlineStr">
+      <c r="BO28" s="1" t="inlineStr">
         <is>
           <t>0.0013</t>
         </is>
       </c>
-      <c r="BO28" s="1" t="inlineStr"/>
       <c r="BP28" s="1" t="inlineStr">
         <is>
           <t>0.160</t>
@@ -9833,7 +9773,7 @@
       </c>
       <c r="C29" s="1" t="inlineStr">
         <is>
-          <t>05/17/2024</t>
+          <t>05/17/24</t>
         </is>
       </c>
       <c r="D29" s="1" t="inlineStr">
@@ -9913,12 +9853,12 @@
       </c>
       <c r="S29" s="1" t="inlineStr">
         <is>
+          <t>0.015</t>
+        </is>
+      </c>
+      <c r="T29" s="1" t="inlineStr">
+        <is>
           <t>0.005</t>
-        </is>
-      </c>
-      <c r="T29" s="1" t="inlineStr">
-        <is>
-          <t>0.015</t>
         </is>
       </c>
       <c r="U29" s="1" t="inlineStr">
@@ -10006,12 +9946,12 @@
       </c>
       <c r="AN29" s="1" t="inlineStr">
         <is>
+          <t>0.014</t>
+        </is>
+      </c>
+      <c r="AO29" s="1" t="inlineStr">
+        <is>
           <t>0.005</t>
-        </is>
-      </c>
-      <c r="AO29" s="1" t="inlineStr">
-        <is>
-          <t>0.014</t>
         </is>
       </c>
       <c r="AP29" s="1" t="inlineStr">
@@ -10087,12 +10027,12 @@
       </c>
       <c r="BE29" s="1" t="inlineStr">
         <is>
+          <t>0.015</t>
+        </is>
+      </c>
+      <c r="BF29" s="1" t="inlineStr">
+        <is>
           <t>0.005</t>
-        </is>
-      </c>
-      <c r="BF29" s="1" t="inlineStr">
-        <is>
-          <t>0.015</t>
         </is>
       </c>
       <c r="BG29" s="1" t="inlineStr">
@@ -10199,7 +10139,7 @@
       </c>
       <c r="C30" s="1" t="inlineStr">
         <is>
-          <t>05/17/2024</t>
+          <t>05/17/24</t>
         </is>
       </c>
       <c r="D30" s="1" t="inlineStr">
@@ -10279,42 +10219,42 @@
       </c>
       <c r="S30" s="1" t="inlineStr">
         <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="T30" s="1" t="inlineStr">
+        <is>
+          <t>0.014</t>
+        </is>
+      </c>
+      <c r="U30" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="V30" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="W30" s="1" t="inlineStr">
+        <is>
+          <t>0.26</t>
+        </is>
+      </c>
+      <c r="X30" s="1" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="Y30" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="Z30" s="1" t="inlineStr">
+        <is>
           <t>0.028</t>
-        </is>
-      </c>
-      <c r="T30" s="1" t="inlineStr">
-        <is>
-          <t>0.014</t>
-        </is>
-      </c>
-      <c r="U30" s="1" t="inlineStr">
-        <is>
-          <t>0.26</t>
-        </is>
-      </c>
-      <c r="V30" s="1" t="inlineStr">
-        <is>
-          <t>0.11</t>
-        </is>
-      </c>
-      <c r="W30" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="X30" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="Y30" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="Z30" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
         </is>
       </c>
       <c r="AA30" s="1" t="inlineStr">
@@ -10372,42 +10312,42 @@
       </c>
       <c r="AN30" s="1" t="inlineStr">
         <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="AO30" s="1" t="inlineStr">
+        <is>
+          <t>0.014</t>
+        </is>
+      </c>
+      <c r="AP30" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AQ30" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="AR30" s="1" t="inlineStr">
+        <is>
+          <t>0.25</t>
+        </is>
+      </c>
+      <c r="AS30" s="1" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="AT30" s="1" t="inlineStr">
+        <is>
+          <t>0.004</t>
+        </is>
+      </c>
+      <c r="AU30" s="1" t="inlineStr">
+        <is>
           <t>0.027</t>
-        </is>
-      </c>
-      <c r="AO30" s="1" t="inlineStr">
-        <is>
-          <t>0.014</t>
-        </is>
-      </c>
-      <c r="AP30" s="1" t="inlineStr">
-        <is>
-          <t>0.25</t>
-        </is>
-      </c>
-      <c r="AQ30" s="1" t="inlineStr">
-        <is>
-          <t>0.11</t>
-        </is>
-      </c>
-      <c r="AR30" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="AS30" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="AT30" s="1" t="inlineStr">
-        <is>
-          <t>0.004</t>
-        </is>
-      </c>
-      <c r="AU30" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
         </is>
       </c>
       <c r="AV30" s="1" t="inlineStr">
@@ -10453,42 +10393,42 @@
       </c>
       <c r="BE30" s="1" t="inlineStr">
         <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="BF30" s="1" t="inlineStr">
+        <is>
+          <t>0.015</t>
+        </is>
+      </c>
+      <c r="BG30" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="BH30" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="BI30" s="1" t="inlineStr">
+        <is>
+          <t>0.24</t>
+        </is>
+      </c>
+      <c r="BJ30" s="1" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="BK30" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="BL30" s="1" t="inlineStr">
+        <is>
           <t>0.026</t>
-        </is>
-      </c>
-      <c r="BF30" s="1" t="inlineStr">
-        <is>
-          <t>0.015</t>
-        </is>
-      </c>
-      <c r="BG30" s="1" t="inlineStr">
-        <is>
-          <t>0.24</t>
-        </is>
-      </c>
-      <c r="BH30" s="1" t="inlineStr">
-        <is>
-          <t>0.12</t>
-        </is>
-      </c>
-      <c r="BI30" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="BJ30" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="BK30" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="BL30" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
         </is>
       </c>
       <c r="BM30" s="1" t="inlineStr">
@@ -10570,7 +10510,7 @@
       </c>
       <c r="D31" s="1" t="inlineStr">
         <is>
-          <t>Berg Pipe Panama City Corp</t>
+          <t>Berg Pipe-Panama City, FL</t>
         </is>
       </c>
       <c r="E31" s="1" t="inlineStr">
@@ -10645,42 +10585,42 @@
       </c>
       <c r="S31" s="1" t="inlineStr">
         <is>
+          <t>0.014</t>
+        </is>
+      </c>
+      <c r="T31" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="U31" s="1" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="V31" s="1" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="W31" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="X31" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="Y31" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="Z31" s="1" t="inlineStr">
+        <is>
           <t>0.029</t>
-        </is>
-      </c>
-      <c r="T31" s="1" t="inlineStr">
-        <is>
-          <t>0.014</t>
-        </is>
-      </c>
-      <c r="U31" s="1" t="inlineStr">
-        <is>
-          <t>0.23</t>
-        </is>
-      </c>
-      <c r="V31" s="1" t="inlineStr">
-        <is>
-          <t>0.09</t>
-        </is>
-      </c>
-      <c r="W31" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="X31" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="Y31" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="Z31" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
         </is>
       </c>
       <c r="AA31" s="1" t="inlineStr">
@@ -10738,42 +10678,42 @@
       </c>
       <c r="AN31" s="1" t="inlineStr">
         <is>
+          <t>0.015</t>
+        </is>
+      </c>
+      <c r="AO31" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="AP31" s="1" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="AQ31" s="1" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="AR31" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="AS31" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AT31" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="AU31" s="1" t="inlineStr">
+        <is>
           <t>0.030</t>
-        </is>
-      </c>
-      <c r="AO31" s="1" t="inlineStr">
-        <is>
-          <t>0.015</t>
-        </is>
-      </c>
-      <c r="AP31" s="1" t="inlineStr">
-        <is>
-          <t>0.22</t>
-        </is>
-      </c>
-      <c r="AQ31" s="1" t="inlineStr">
-        <is>
-          <t>0.09</t>
-        </is>
-      </c>
-      <c r="AR31" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="AS31" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="AT31" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="AU31" s="1" t="inlineStr">
-        <is>
-          <t>0.30</t>
         </is>
       </c>
       <c r="AV31" s="1" t="inlineStr">
@@ -10819,42 +10759,42 @@
       </c>
       <c r="BE31" s="1" t="inlineStr">
         <is>
+          <t>0.015</t>
+        </is>
+      </c>
+      <c r="BF31" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="BG31" s="1" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="BH31" s="1" t="inlineStr">
+        <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="BI31" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="BJ31" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="BK31" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="BL31" s="1" t="inlineStr">
+        <is>
           <t>0.030</t>
-        </is>
-      </c>
-      <c r="BF31" s="1" t="inlineStr">
-        <is>
-          <t>0.015</t>
-        </is>
-      </c>
-      <c r="BG31" s="1" t="inlineStr">
-        <is>
-          <t>0.22</t>
-        </is>
-      </c>
-      <c r="BH31" s="1" t="inlineStr">
-        <is>
-          <t>0.09</t>
-        </is>
-      </c>
-      <c r="BI31" s="1" t="inlineStr">
-        <is>
-          <t>0.16</t>
-        </is>
-      </c>
-      <c r="BJ31" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="BK31" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="BL31" s="1" t="inlineStr">
-        <is>
-          <t>0.30</t>
         </is>
       </c>
       <c r="BM31" s="1" t="inlineStr">
@@ -11021,12 +10961,12 @@
       </c>
       <c r="U32" s="1" t="inlineStr">
         <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="V32" s="1" t="inlineStr">
+        <is>
           <t>0.25</t>
-        </is>
-      </c>
-      <c r="V32" s="1" t="inlineStr">
-        <is>
-          <t>0.10</t>
         </is>
       </c>
       <c r="W32" s="1" t="inlineStr">
@@ -11114,12 +11054,12 @@
       </c>
       <c r="AP32" s="1" t="inlineStr">
         <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="AQ32" s="1" t="inlineStr">
+        <is>
           <t>0.24</t>
-        </is>
-      </c>
-      <c r="AQ32" s="1" t="inlineStr">
-        <is>
-          <t>0.09</t>
         </is>
       </c>
       <c r="AR32" s="1" t="inlineStr">
@@ -11195,12 +11135,12 @@
       </c>
       <c r="BG32" s="1" t="inlineStr">
         <is>
+          <t>0.09</t>
+        </is>
+      </c>
+      <c r="BH32" s="1" t="inlineStr">
+        <is>
           <t>0.24</t>
-        </is>
-      </c>
-      <c r="BH32" s="1" t="inlineStr">
-        <is>
-          <t>0.09</t>
         </is>
       </c>
       <c r="BI32" s="1" t="inlineStr">
@@ -11302,7 +11242,7 @@
       </c>
       <c r="D33" s="1" t="inlineStr">
         <is>
-          <t>Berg Pipe-Panama City, FL</t>
+          <t>Berg Pipe Panama City Corp</t>
         </is>
       </c>
       <c r="E33" s="1" t="inlineStr">
@@ -11402,7 +11342,7 @@
       </c>
       <c r="X33" s="1" t="inlineStr">
         <is>
-          <t>0.29</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="Y33" s="1" t="inlineStr">
@@ -11412,7 +11352,7 @@
       </c>
       <c r="Z33" s="1" t="inlineStr">
         <is>
-          <t>0.015</t>
+          <t>0.029</t>
         </is>
       </c>
       <c r="AA33" s="1" t="inlineStr">
@@ -11495,7 +11435,7 @@
       </c>
       <c r="AS33" s="1" t="inlineStr">
         <is>
-          <t>0.29</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="AT33" s="1" t="inlineStr">
@@ -11505,7 +11445,7 @@
       </c>
       <c r="AU33" s="1" t="inlineStr">
         <is>
-          <t>0.015</t>
+          <t>0.029</t>
         </is>
       </c>
       <c r="AV33" s="1" t="inlineStr">
@@ -11576,7 +11516,7 @@
       </c>
       <c r="BJ33" s="1" t="inlineStr">
         <is>
-          <t>0.30</t>
+          <t>0.16</t>
         </is>
       </c>
       <c r="BK33" s="1" t="inlineStr">
@@ -11586,7 +11526,7 @@
       </c>
       <c r="BL33" s="1" t="inlineStr">
         <is>
-          <t>0.017</t>
+          <t>0.030</t>
         </is>
       </c>
       <c r="BM33" s="1" t="inlineStr">
@@ -11663,7 +11603,7 @@
       </c>
       <c r="C34" s="1" t="inlineStr">
         <is>
-          <t>05/17/24</t>
+          <t>05/17/2024</t>
         </is>
       </c>
       <c r="D34" s="1" t="inlineStr">
@@ -12034,7 +11974,7 @@
       </c>
       <c r="D35" s="1" t="inlineStr">
         <is>
-          <t>Berg Pipe-Panama City, FL</t>
+          <t>Berg Pipe Panama City Corp</t>
         </is>
       </c>
       <c r="E35" s="1" t="inlineStr">
@@ -12119,49 +12059,45 @@
       </c>
       <c r="U35" s="1" t="inlineStr">
         <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="V35" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="W35" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="X35" s="1" t="inlineStr">
+        <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="Y35" s="1" t="inlineStr">
+        <is>
           <t>0.12</t>
         </is>
       </c>
-      <c r="V35" s="1" t="inlineStr">
+      <c r="Z35" s="1" t="inlineStr">
         <is>
           <t>0.0002</t>
         </is>
       </c>
-      <c r="W35" s="1" t="inlineStr">
+      <c r="AA35" s="1" t="inlineStr">
         <is>
           <t>0.008</t>
         </is>
       </c>
-      <c r="X35" s="1" t="inlineStr">
+      <c r="AB35" s="1" t="inlineStr">
         <is>
           <t>0.0013</t>
         </is>
       </c>
-      <c r="Y35" s="1" t="inlineStr">
-        <is>
-          <t>0.029</t>
-        </is>
-      </c>
-      <c r="Z35" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="AA35" s="1" t="inlineStr">
-        <is>
-          <t>0.0002</t>
-        </is>
-      </c>
-      <c r="AB35" s="1" t="inlineStr">
-        <is>
-          <t>0.008</t>
-        </is>
-      </c>
-      <c r="AC35" s="1" t="inlineStr">
-        <is>
-          <t>0.0013</t>
-        </is>
-      </c>
+      <c r="AC35" s="1" t="inlineStr"/>
       <c r="AD35" s="1" t="inlineStr">
         <is>
           <t>0.362</t>
@@ -12212,49 +12148,45 @@
       </c>
       <c r="AP35" s="1" t="inlineStr">
         <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="AQ35" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="AR35" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="AS35" s="1" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="AT35" s="1" t="inlineStr">
+        <is>
           <t>0.12</t>
         </is>
       </c>
-      <c r="AQ35" s="1" t="inlineStr">
+      <c r="AU35" s="1" t="inlineStr">
         <is>
           <t>0.0001</t>
         </is>
       </c>
-      <c r="AR35" s="1" t="inlineStr">
+      <c r="AV35" s="1" t="inlineStr">
         <is>
           <t>0.009</t>
         </is>
       </c>
-      <c r="AS35" s="1" t="inlineStr">
+      <c r="AW35" s="1" t="inlineStr">
         <is>
           <t>0.0012</t>
         </is>
       </c>
-      <c r="AT35" s="1" t="inlineStr">
-        <is>
-          <t>0.027</t>
-        </is>
-      </c>
-      <c r="AU35" s="1" t="inlineStr">
-        <is>
-          <t>0.29</t>
-        </is>
-      </c>
-      <c r="AV35" s="1" t="inlineStr">
-        <is>
-          <t>0.0001</t>
-        </is>
-      </c>
-      <c r="AW35" s="1" t="inlineStr">
-        <is>
-          <t>0.009</t>
-        </is>
-      </c>
-      <c r="AX35" s="1" t="inlineStr">
-        <is>
-          <t>0.0012</t>
-        </is>
-      </c>
+      <c r="AX35" s="1" t="inlineStr"/>
       <c r="AY35" s="1" t="inlineStr"/>
       <c r="AZ35" s="1" t="inlineStr">
         <is>
@@ -12293,49 +12225,45 @@
       </c>
       <c r="BG35" s="1" t="inlineStr">
         <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="BH35" s="1" t="inlineStr">
+        <is>
+          <t>0.16</t>
+        </is>
+      </c>
+      <c r="BI35" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="BJ35" s="1" t="inlineStr">
+        <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="BK35" s="1" t="inlineStr">
+        <is>
           <t>0.12</t>
         </is>
       </c>
-      <c r="BH35" s="1" t="inlineStr">
+      <c r="BL35" s="1" t="inlineStr">
         <is>
           <t>0.0001</t>
         </is>
       </c>
-      <c r="BI35" s="1" t="inlineStr">
+      <c r="BM35" s="1" t="inlineStr">
         <is>
           <t>0.009</t>
         </is>
       </c>
-      <c r="BJ35" s="1" t="inlineStr">
+      <c r="BN35" s="1" t="inlineStr">
         <is>
           <t>0.0014</t>
         </is>
       </c>
-      <c r="BK35" s="1" t="inlineStr">
-        <is>
-          <t>0.028</t>
-        </is>
-      </c>
-      <c r="BL35" s="1" t="inlineStr">
-        <is>
-          <t>0.28</t>
-        </is>
-      </c>
-      <c r="BM35" s="1" t="inlineStr">
-        <is>
-          <t>0.0001</t>
-        </is>
-      </c>
-      <c r="BN35" s="1" t="inlineStr">
-        <is>
-          <t>0.009</t>
-        </is>
-      </c>
-      <c r="BO35" s="1" t="inlineStr">
-        <is>
-          <t>0.0014</t>
-        </is>
-      </c>
+      <c r="BO35" s="1" t="inlineStr"/>
       <c r="BP35" s="1" t="inlineStr">
         <is>
           <t>0.354</t>
@@ -12761,7 +12689,7 @@
       </c>
       <c r="C37" s="1" t="inlineStr">
         <is>
-          <t>05/17/24</t>
+          <t>05/17/2024</t>
         </is>
       </c>
       <c r="D37" s="1" t="inlineStr">
@@ -12866,7 +12794,7 @@
       </c>
       <c r="X37" s="1" t="inlineStr">
         <is>
-          <t>0.16</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="Y37" s="1" t="inlineStr">
@@ -12876,7 +12804,7 @@
       </c>
       <c r="Z37" s="1" t="inlineStr">
         <is>
-          <t>0.029</t>
+          <t>0.016</t>
         </is>
       </c>
       <c r="AA37" s="1" t="inlineStr">
@@ -12959,7 +12887,7 @@
       </c>
       <c r="AS37" s="1" t="inlineStr">
         <is>
-          <t>0.16</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="AT37" s="1" t="inlineStr">
@@ -12969,7 +12897,7 @@
       </c>
       <c r="AU37" s="1" t="inlineStr">
         <is>
-          <t>0.029</t>
+          <t>0.016</t>
         </is>
       </c>
       <c r="AV37" s="1" t="inlineStr">
@@ -13040,7 +12968,7 @@
       </c>
       <c r="BJ37" s="1" t="inlineStr">
         <is>
-          <t>0.16</t>
+          <t>0.29</t>
         </is>
       </c>
       <c r="BK37" s="1" t="inlineStr">
@@ -13050,7 +12978,7 @@
       </c>
       <c r="BL37" s="1" t="inlineStr">
         <is>
-          <t>0.032</t>
+          <t>0.015</t>
         </is>
       </c>
       <c r="BM37" s="1" t="inlineStr">
@@ -13132,7 +13060,7 @@
       </c>
       <c r="D38" s="1" t="inlineStr">
         <is>
-          <t>Berg Pipe-Panama City, FL</t>
+          <t>Berg Pipe Panama City Corp</t>
         </is>
       </c>
       <c r="E38" s="1" t="inlineStr">
@@ -13217,32 +13145,32 @@
       </c>
       <c r="U38" s="1" t="inlineStr">
         <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="V38" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="W38" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="X38" s="1" t="inlineStr">
+        <is>
           <t>0.22</t>
         </is>
       </c>
-      <c r="V38" s="1" t="inlineStr">
+      <c r="Y38" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="Z38" s="1" t="inlineStr">
         <is>
           <t>0.10</t>
-        </is>
-      </c>
-      <c r="W38" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="X38" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="Y38" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="Z38" s="1" t="inlineStr">
-        <is>
-          <t>0.030</t>
         </is>
       </c>
       <c r="AA38" s="1" t="inlineStr">
@@ -13310,32 +13238,32 @@
       </c>
       <c r="AP38" s="1" t="inlineStr">
         <is>
+          <t>0.29</t>
+        </is>
+      </c>
+      <c r="AQ38" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="AR38" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="AS38" s="1" t="inlineStr">
+        <is>
           <t>0.21</t>
         </is>
       </c>
-      <c r="AQ38" s="1" t="inlineStr">
+      <c r="AT38" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="AU38" s="1" t="inlineStr">
         <is>
           <t>0.10</t>
-        </is>
-      </c>
-      <c r="AR38" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="AS38" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="AT38" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="AU38" s="1" t="inlineStr">
-        <is>
-          <t>0.030</t>
         </is>
       </c>
       <c r="AV38" s="1" t="inlineStr">
@@ -13391,32 +13319,32 @@
       </c>
       <c r="BG38" s="1" t="inlineStr">
         <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="BH38" s="1" t="inlineStr">
+        <is>
+          <t>0.17</t>
+        </is>
+      </c>
+      <c r="BI38" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="BJ38" s="1" t="inlineStr">
+        <is>
           <t>0.22</t>
         </is>
       </c>
-      <c r="BH38" s="1" t="inlineStr">
+      <c r="BK38" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="BL38" s="1" t="inlineStr">
         <is>
           <t>0.09</t>
-        </is>
-      </c>
-      <c r="BI38" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="BJ38" s="1" t="inlineStr">
-        <is>
-          <t>0.17</t>
-        </is>
-      </c>
-      <c r="BK38" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="BL38" s="1" t="inlineStr">
-        <is>
-          <t>0.030</t>
         </is>
       </c>
       <c r="BM38" s="1" t="inlineStr">
@@ -13498,7 +13426,7 @@
       </c>
       <c r="D39" s="1" t="inlineStr">
         <is>
-          <t>Berg Pipe Panama City Corp</t>
+          <t>Berg Pipe-Panama City, FL</t>
         </is>
       </c>
       <c r="E39" s="1" t="inlineStr">
@@ -13608,7 +13536,7 @@
       </c>
       <c r="Z39" s="1" t="inlineStr">
         <is>
-          <t>0.10</t>
+          <t>0.010</t>
         </is>
       </c>
       <c r="AA39" s="1" t="inlineStr">
@@ -13701,7 +13629,7 @@
       </c>
       <c r="AU39" s="1" t="inlineStr">
         <is>
-          <t>0.09</t>
+          <t>0.009</t>
         </is>
       </c>
       <c r="AV39" s="1" t="inlineStr">
@@ -13782,7 +13710,7 @@
       </c>
       <c r="BL39" s="1" t="inlineStr">
         <is>
-          <t>0.09</t>
+          <t>0.009</t>
         </is>
       </c>
       <c r="BM39" s="1" t="inlineStr">
@@ -13859,7 +13787,7 @@
       </c>
       <c r="C40" s="1" t="inlineStr">
         <is>
-          <t>05/17/2024</t>
+          <t>05/17/24</t>
         </is>
       </c>
       <c r="D40" s="1" t="inlineStr">
@@ -13959,12 +13887,12 @@
       </c>
       <c r="W40" s="1" t="inlineStr">
         <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="X40" s="1" t="inlineStr">
+        <is>
           <t>0.17</t>
-        </is>
-      </c>
-      <c r="X40" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
         </is>
       </c>
       <c r="Y40" s="1" t="inlineStr">
@@ -14052,12 +13980,12 @@
       </c>
       <c r="AR40" s="1" t="inlineStr">
         <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="AS40" s="1" t="inlineStr">
+        <is>
           <t>0.17</t>
-        </is>
-      </c>
-      <c r="AS40" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
         </is>
       </c>
       <c r="AT40" s="1" t="inlineStr">
@@ -14133,12 +14061,12 @@
       </c>
       <c r="BI40" s="1" t="inlineStr">
         <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="BJ40" s="1" t="inlineStr">
+        <is>
           <t>0.16</t>
-        </is>
-      </c>
-      <c r="BJ40" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
         </is>
       </c>
       <c r="BK40" s="1" t="inlineStr">
@@ -14230,7 +14158,7 @@
       </c>
       <c r="D41" s="1" t="inlineStr">
         <is>
-          <t>Berg Pipe-Panama City, FL</t>
+          <t>Berg Pipe Panama City Corp</t>
         </is>
       </c>
       <c r="E41" s="1" t="inlineStr">
@@ -14671,42 +14599,42 @@
       </c>
       <c r="S42" s="1" t="inlineStr">
         <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="T42" s="1" t="inlineStr">
+        <is>
           <t>0.012</t>
         </is>
       </c>
-      <c r="T42" s="1" t="inlineStr">
+      <c r="U42" s="1" t="inlineStr">
+        <is>
+          <t>0.22</t>
+        </is>
+      </c>
+      <c r="V42" s="1" t="inlineStr">
+        <is>
+          <t>0.11</t>
+        </is>
+      </c>
+      <c r="W42" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="X42" s="1" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="Y42" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="Z42" s="1" t="inlineStr">
         <is>
           <t>0.025</t>
-        </is>
-      </c>
-      <c r="U42" s="1" t="inlineStr">
-        <is>
-          <t>0.22</t>
-        </is>
-      </c>
-      <c r="V42" s="1" t="inlineStr">
-        <is>
-          <t>0.11</t>
-        </is>
-      </c>
-      <c r="W42" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="X42" s="1" t="inlineStr">
-        <is>
-          <t>0.18</t>
-        </is>
-      </c>
-      <c r="Y42" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="Z42" s="1" t="inlineStr">
-        <is>
-          <t>0.012</t>
         </is>
       </c>
       <c r="AA42" s="1" t="inlineStr">
@@ -14764,42 +14692,42 @@
       </c>
       <c r="AN42" s="1" t="inlineStr">
         <is>
+          <t>0.27</t>
+        </is>
+      </c>
+      <c r="AO42" s="1" t="inlineStr">
+        <is>
           <t>0.011</t>
         </is>
       </c>
-      <c r="AO42" s="1" t="inlineStr">
+      <c r="AP42" s="1" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="AQ42" s="1" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="AR42" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="AS42" s="1" t="inlineStr">
+        <is>
+          <t>0.18</t>
+        </is>
+      </c>
+      <c r="AT42" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="AU42" s="1" t="inlineStr">
         <is>
           <t>0.025</t>
-        </is>
-      </c>
-      <c r="AP42" s="1" t="inlineStr">
-        <is>
-          <t>0.23</t>
-        </is>
-      </c>
-      <c r="AQ42" s="1" t="inlineStr">
-        <is>
-          <t>0.12</t>
-        </is>
-      </c>
-      <c r="AR42" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="AS42" s="1" t="inlineStr">
-        <is>
-          <t>0.18</t>
-        </is>
-      </c>
-      <c r="AT42" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="AU42" s="1" t="inlineStr">
-        <is>
-          <t>0.011</t>
         </is>
       </c>
       <c r="AV42" s="1" t="inlineStr">
@@ -14845,42 +14773,42 @@
       </c>
       <c r="BE42" s="1" t="inlineStr">
         <is>
+          <t>0.28</t>
+        </is>
+      </c>
+      <c r="BF42" s="1" t="inlineStr">
+        <is>
           <t>0.012</t>
         </is>
       </c>
-      <c r="BF42" s="1" t="inlineStr">
+      <c r="BG42" s="1" t="inlineStr">
+        <is>
+          <t>0.23</t>
+        </is>
+      </c>
+      <c r="BH42" s="1" t="inlineStr">
+        <is>
+          <t>0.12</t>
+        </is>
+      </c>
+      <c r="BI42" s="1" t="inlineStr">
+        <is>
+          <t>0.06</t>
+        </is>
+      </c>
+      <c r="BJ42" s="1" t="inlineStr">
+        <is>
+          <t>0.19</t>
+        </is>
+      </c>
+      <c r="BK42" s="1" t="inlineStr">
+        <is>
+          <t>0.005</t>
+        </is>
+      </c>
+      <c r="BL42" s="1" t="inlineStr">
         <is>
           <t>0.026</t>
-        </is>
-      </c>
-      <c r="BG42" s="1" t="inlineStr">
-        <is>
-          <t>0.23</t>
-        </is>
-      </c>
-      <c r="BH42" s="1" t="inlineStr">
-        <is>
-          <t>0.12</t>
-        </is>
-      </c>
-      <c r="BI42" s="1" t="inlineStr">
-        <is>
-          <t>0.06</t>
-        </is>
-      </c>
-      <c r="BJ42" s="1" t="inlineStr">
-        <is>
-          <t>0.19</t>
-        </is>
-      </c>
-      <c r="BK42" s="1" t="inlineStr">
-        <is>
-          <t>0.005</t>
-        </is>
-      </c>
-      <c r="BL42" s="1" t="inlineStr">
-        <is>
-          <t>0.012</t>
         </is>
       </c>
       <c r="BM42" s="1" t="inlineStr">

</xml_diff>

<commit_message>
Modularization: add mtr_processor package and CLIs; redirect outputs to output/; add rotating loggers; update uploader defaults; update README; ignore logs and output; move JSONs out of Sample json
</commit_message>
<xml_diff>
--- a/Sample json/NEW_.xlsx
+++ b/Sample json/NEW_.xlsx
@@ -861,7 +861,7 @@
       </c>
       <c r="G3" s="1" t="inlineStr">
         <is>
-          <t>70900</t>
+          <t>75400</t>
         </is>
       </c>
       <c r="H3" s="1" t="inlineStr">
@@ -871,7 +871,7 @@
       </c>
       <c r="I3" s="1" t="inlineStr">
         <is>
-          <t>75400</t>
+          <t>83600</t>
         </is>
       </c>
       <c r="J3" s="1" t="inlineStr">

</xml_diff>